<commit_message>
add * to required feilad
</commit_message>
<xml_diff>
--- a/public/assets/website.xlsx
+++ b/public/assets/website.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Website Url</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Link Insertion Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insertion currency</t>
   </si>
   <si>
     <t xml:space="preserve">DR</t>
@@ -82,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,6 +107,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,25 +178,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -243,7 +249,10 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>